<commit_message>
COTS POC RAPID Notebook
</commit_message>
<xml_diff>
--- a/images/POC_gDNA_mtORF_Plates.xlsx
+++ b/images/POC_gDNA_mtORF_Plates.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Putnam_Lab_Notebook/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634B0E30-4320-2F4B-A82A-78F58B0C3584}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A11E999-15C2-EA4C-B6CF-43024BF004F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{EBCD61C8-57A8-CD45-8415-F852AB071768}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="25700" windowHeight="13900" xr2:uid="{EBCD61C8-57A8-CD45-8415-F852AB071768}"/>
   </bookViews>
   <sheets>
     <sheet name="20240412_Plate001" sheetId="1" r:id="rId1"/>
+    <sheet name="Plate002" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'20240412_Plate001'!$A$13:$M$29</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="219">
   <si>
     <t>Reagent</t>
   </si>
@@ -400,13 +401,304 @@
   </si>
   <si>
     <t>Zymo Kit did not have enough Genomic lysis buffer for these samples</t>
+  </si>
+  <si>
+    <t>Plate 002 gDNA Extraction</t>
+  </si>
+  <si>
+    <t>TPC REC-037</t>
+  </si>
+  <si>
+    <t>TPC REC-038</t>
+  </si>
+  <si>
+    <t>TPC REC-039</t>
+  </si>
+  <si>
+    <t>TPC REC-040</t>
+  </si>
+  <si>
+    <t>S5T6 - 1373</t>
+  </si>
+  <si>
+    <t>S1T3 - 1274</t>
+  </si>
+  <si>
+    <t>S1T3 - 1314</t>
+  </si>
+  <si>
+    <t>S1T4 - 1281</t>
+  </si>
+  <si>
+    <t>S1T3 - 1347</t>
+  </si>
+  <si>
+    <t>S1T3 - 1271</t>
+  </si>
+  <si>
+    <t>S1T1 - 1244</t>
+  </si>
+  <si>
+    <t>S1T1 - 1258</t>
+  </si>
+  <si>
+    <t>S5T6 - 1370</t>
+  </si>
+  <si>
+    <t>S1T3 - 1275</t>
+  </si>
+  <si>
+    <t>Plate 001 mtOTF Sanger</t>
+  </si>
+  <si>
+    <t>HP_001</t>
+  </si>
+  <si>
+    <t>HP_002</t>
+  </si>
+  <si>
+    <t>HP_003</t>
+  </si>
+  <si>
+    <t>HP_004</t>
+  </si>
+  <si>
+    <t>HP_005</t>
+  </si>
+  <si>
+    <t>HP_006</t>
+  </si>
+  <si>
+    <t>HP_007</t>
+  </si>
+  <si>
+    <t>HP_008</t>
+  </si>
+  <si>
+    <t>HP_009</t>
+  </si>
+  <si>
+    <t>HP_010</t>
+  </si>
+  <si>
+    <t>HP_011</t>
+  </si>
+  <si>
+    <t>HP_012</t>
+  </si>
+  <si>
+    <t>HP_013</t>
+  </si>
+  <si>
+    <t>HP_014</t>
+  </si>
+  <si>
+    <t>HP_015</t>
+  </si>
+  <si>
+    <t>HP_016</t>
+  </si>
+  <si>
+    <t>HP_017</t>
+  </si>
+  <si>
+    <t>HP_018</t>
+  </si>
+  <si>
+    <t>HP_019</t>
+  </si>
+  <si>
+    <t>HP_020</t>
+  </si>
+  <si>
+    <t>HP_021</t>
+  </si>
+  <si>
+    <t>HP_022</t>
+  </si>
+  <si>
+    <t>HP_023</t>
+  </si>
+  <si>
+    <t>HP_024</t>
+  </si>
+  <si>
+    <t>HP_025</t>
+  </si>
+  <si>
+    <t>HP_026</t>
+  </si>
+  <si>
+    <t>HP_027</t>
+  </si>
+  <si>
+    <t>HP_028</t>
+  </si>
+  <si>
+    <t>HP_029</t>
+  </si>
+  <si>
+    <t>HP_030</t>
+  </si>
+  <si>
+    <t>HP_031</t>
+  </si>
+  <si>
+    <t>HP_032</t>
+  </si>
+  <si>
+    <t>HP_033</t>
+  </si>
+  <si>
+    <t>HP_034</t>
+  </si>
+  <si>
+    <t>HP_035</t>
+  </si>
+  <si>
+    <t>HP_036</t>
+  </si>
+  <si>
+    <t>HP_037</t>
+  </si>
+  <si>
+    <t>HP_038</t>
+  </si>
+  <si>
+    <t>HP_039</t>
+  </si>
+  <si>
+    <t>HP_040</t>
+  </si>
+  <si>
+    <t>HP_041</t>
+  </si>
+  <si>
+    <t>HP_042</t>
+  </si>
+  <si>
+    <t>HP_043</t>
+  </si>
+  <si>
+    <t>HP_044</t>
+  </si>
+  <si>
+    <t>HP_045</t>
+  </si>
+  <si>
+    <t>HP_046</t>
+  </si>
+  <si>
+    <t>HP_047</t>
+  </si>
+  <si>
+    <t>HP_048</t>
+  </si>
+  <si>
+    <t>HP_049</t>
+  </si>
+  <si>
+    <t>HP_050</t>
+  </si>
+  <si>
+    <t>HP_051</t>
+  </si>
+  <si>
+    <t>HP_052</t>
+  </si>
+  <si>
+    <t>HP_053</t>
+  </si>
+  <si>
+    <t>HP_054</t>
+  </si>
+  <si>
+    <t>HP_055</t>
+  </si>
+  <si>
+    <t>HP_056</t>
+  </si>
+  <si>
+    <t>HP_057</t>
+  </si>
+  <si>
+    <t>HP_058</t>
+  </si>
+  <si>
+    <t>HP_059</t>
+  </si>
+  <si>
+    <t>HP_060</t>
+  </si>
+  <si>
+    <t>HP_061</t>
+  </si>
+  <si>
+    <t>HP_062</t>
+  </si>
+  <si>
+    <t>HP_063</t>
+  </si>
+  <si>
+    <t>HP_064</t>
+  </si>
+  <si>
+    <t>HP_065</t>
+  </si>
+  <si>
+    <t>HP_066</t>
+  </si>
+  <si>
+    <t>HP_067</t>
+  </si>
+  <si>
+    <t>HP_068</t>
+  </si>
+  <si>
+    <t>HP_069</t>
+  </si>
+  <si>
+    <t>HP_070</t>
+  </si>
+  <si>
+    <t>HP_071</t>
+  </si>
+  <si>
+    <t>HP_072</t>
+  </si>
+  <si>
+    <t>HP_073</t>
+  </si>
+  <si>
+    <t>HP_074</t>
+  </si>
+  <si>
+    <t>HP_075</t>
+  </si>
+  <si>
+    <t>HP_076</t>
+  </si>
+  <si>
+    <t>HP_077</t>
+  </si>
+  <si>
+    <t>HP_078</t>
+  </si>
+  <si>
+    <t>HP_079</t>
+  </si>
+  <si>
+    <t>HP_080</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -468,6 +760,13 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -543,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -581,6 +880,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,10 +1212,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1757,6 +2071,375 @@
         <v>120</v>
       </c>
     </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8">
+        <v>2</v>
+      </c>
+      <c r="D32" s="8">
+        <v>3</v>
+      </c>
+      <c r="E32" s="8">
+        <v>4</v>
+      </c>
+      <c r="F32" s="8">
+        <v>5</v>
+      </c>
+      <c r="G32" s="8">
+        <v>6</v>
+      </c>
+      <c r="H32" s="8">
+        <v>7</v>
+      </c>
+      <c r="I32" s="8">
+        <v>8</v>
+      </c>
+      <c r="J32" s="8">
+        <v>9</v>
+      </c>
+      <c r="K32" s="8">
+        <v>10</v>
+      </c>
+      <c r="L32" s="8">
+        <v>11</v>
+      </c>
+      <c r="M32" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="I33" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="K33" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="K34" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="J35" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="K35" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I36" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="K36" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="J37" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="K37" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="K38" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="I39" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="K39" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="K40" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="L10:M10"/>
@@ -1766,4 +2449,513 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CC85F7-C1B0-5C40-8562-B4850301C85D}">
+  <dimension ref="A1:O30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40" style="5" customWidth="1"/>
+    <col min="2" max="13" width="9.6640625" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="8">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8">
+        <v>9</v>
+      </c>
+      <c r="K1" s="8">
+        <v>10</v>
+      </c>
+      <c r="L1" s="8">
+        <v>11</v>
+      </c>
+      <c r="M1" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="N2" s="17"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="18"/>
+    </row>
+    <row r="7" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="18"/>
+    </row>
+    <row r="8" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="18"/>
+    </row>
+    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="12" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="C14" s="4">
+        <f>B14*85</f>
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" ref="C15:C19" si="0">B15*85</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="4">
+        <v>10.9</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>926.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2</v>
+      </c>
+      <c r="D21" s="8">
+        <v>3</v>
+      </c>
+      <c r="E21" s="8">
+        <v>4</v>
+      </c>
+      <c r="F21" s="8">
+        <v>5</v>
+      </c>
+      <c r="G21" s="8">
+        <v>6</v>
+      </c>
+      <c r="H21" s="8">
+        <v>7</v>
+      </c>
+      <c r="I21" s="8">
+        <v>8</v>
+      </c>
+      <c r="J21" s="8">
+        <v>9</v>
+      </c>
+      <c r="K21" s="8">
+        <v>10</v>
+      </c>
+      <c r="L21" s="8">
+        <v>11</v>
+      </c>
+      <c r="M21" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="1:13" ht="24" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N2:N9"/>
+    <mergeCell ref="L10:M10"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating notebook for sanger setup plates 002 and 003
</commit_message>
<xml_diff>
--- a/images/POC_gDNA_mtORF_Plates.xlsx
+++ b/images/POC_gDNA_mtORF_Plates.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Putnam_Lab_Notebook/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D70A09-DE9A-244B-A00B-0FF2EFE0686B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F06BD58-7ECC-4E47-8E50-55CE0FD74271}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="18640" windowHeight="13860" activeTab="1" xr2:uid="{EBCD61C8-57A8-CD45-8415-F852AB071768}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="3" xr2:uid="{EBCD61C8-57A8-CD45-8415-F852AB071768}"/>
   </bookViews>
   <sheets>
     <sheet name="20240412_Plate001" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Plate002" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'20240412_Plate001'!$A$13:$M$29</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="316">
   <si>
     <t>Reagent</t>
   </si>
@@ -981,6 +982,9 @@
   </si>
   <si>
     <t>H12</t>
+  </si>
+  <si>
+    <t>Plate          gDNA Extraction</t>
   </si>
 </sst>
 </file>
@@ -1159,22 +1163,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1183,6 +1171,22 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1503,14 +1507,16 @@
   </sheetPr>
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B40"/>
+    <sheetView topLeftCell="A29" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" style="5" customWidth="1"/>
-    <col min="2" max="13" width="9.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15" style="5" customWidth="1"/>
+    <col min="4" max="13" width="9.6640625" style="5" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
@@ -1595,7 +1601,7 @@
       <c r="M2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="18" t="s">
         <v>121</v>
       </c>
       <c r="O2" s="12"/>
@@ -1640,7 +1646,7 @@
       <c r="M3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="14"/>
+      <c r="N3" s="19"/>
     </row>
     <row r="4" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
@@ -1682,7 +1688,7 @@
       <c r="M4" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="14"/>
+      <c r="N4" s="19"/>
     </row>
     <row r="5" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -1724,7 +1730,7 @@
       <c r="M5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="N5" s="14"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
@@ -1766,7 +1772,7 @@
       <c r="M6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="N6" s="14"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -1808,7 +1814,7 @@
       <c r="M7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="N7" s="14"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1850,7 +1856,7 @@
       <c r="M8" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="N8" s="14"/>
+      <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
@@ -1892,11 +1898,11 @@
       <c r="M9" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="N9" s="14"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L10" s="15"/>
-      <c r="M10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -2420,19 +2426,19 @@
       <c r="F33" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="I33" s="21" t="s">
+      <c r="I33" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="J33" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="K33" s="21" t="s">
+      <c r="K33" s="15" t="s">
         <v>210</v>
       </c>
       <c r="L33" s="6" t="s">
@@ -2461,19 +2467,19 @@
       <c r="F34" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="H34" s="21" t="s">
+      <c r="H34" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="I34" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="J34" s="21" t="s">
+      <c r="J34" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="K34" s="21" t="s">
+      <c r="K34" s="15" t="s">
         <v>211</v>
       </c>
       <c r="L34" s="6" t="s">
@@ -2502,19 +2508,19 @@
       <c r="F35" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I35" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="J35" s="21" t="s">
+      <c r="J35" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="K35" s="21" t="s">
+      <c r="K35" s="15" t="s">
         <v>212</v>
       </c>
       <c r="L35" s="6" t="s">
@@ -2543,19 +2549,19 @@
       <c r="F36" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="H36" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="I36" s="21" t="s">
+      <c r="I36" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="J36" s="21" t="s">
+      <c r="J36" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="K36" s="21" t="s">
+      <c r="K36" s="15" t="s">
         <v>213</v>
       </c>
       <c r="L36" s="6" t="s">
@@ -2584,19 +2590,19 @@
       <c r="F37" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="H37" s="21" t="s">
+      <c r="H37" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="I37" s="21" t="s">
+      <c r="I37" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="J37" s="21" t="s">
+      <c r="J37" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="K37" s="21" t="s">
+      <c r="K37" s="15" t="s">
         <v>214</v>
       </c>
       <c r="L37" s="6" t="s">
@@ -2625,19 +2631,19 @@
       <c r="F38" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="H38" s="21" t="s">
+      <c r="H38" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="I38" s="21" t="s">
+      <c r="I38" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="J38" s="21" t="s">
+      <c r="J38" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="K38" s="21" t="s">
+      <c r="K38" s="15" t="s">
         <v>215</v>
       </c>
       <c r="L38" s="6" t="s">
@@ -2666,19 +2672,19 @@
       <c r="F39" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G39" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="H39" s="21" t="s">
+      <c r="H39" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="I39" s="21" t="s">
+      <c r="I39" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="J39" s="21" t="s">
+      <c r="J39" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="K39" s="21" t="s">
+      <c r="K39" s="15" t="s">
         <v>216</v>
       </c>
       <c r="L39" s="6" t="s">
@@ -2707,19 +2713,19 @@
       <c r="F40" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="I40" s="21" t="s">
+      <c r="I40" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="J40" s="21" t="s">
+      <c r="J40" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="K40" s="21" t="s">
+      <c r="K40" s="15" t="s">
         <v>217</v>
       </c>
       <c r="L40" s="6" t="s">
@@ -2744,8 +2750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595CC3FF-5B2A-C941-8078-A908B7C89D2B}">
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3543,13 +3549,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CC85F7-C1B0-5C40-8562-B4850301C85D}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" style="5" customWidth="1"/>
     <col min="2" max="13" width="9.6640625" style="5" customWidth="1"/>
@@ -3601,180 +3607,180 @@
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="N2" s="17"/>
+      <c r="N2" s="20"/>
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="N3" s="18"/>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="18"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="18"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="18"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="18"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="18"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="18"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="21"/>
     </row>
     <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L10" s="15"/>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="12" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -4039,7 +4045,6 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" ht="24" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="N2:N9"/>
@@ -4048,4 +4053,382 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A51485-E87A-B441-85FD-14A56F30A95E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="A1:M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="2" max="13" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" s="8">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8">
+        <v>9</v>
+      </c>
+      <c r="K1" s="8">
+        <v>10</v>
+      </c>
+      <c r="L1" s="8">
+        <v>11</v>
+      </c>
+      <c r="M1" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+    </row>
+    <row r="5" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" ht="37" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="F11" s="8">
+        <v>5</v>
+      </c>
+      <c r="G11" s="8">
+        <v>6</v>
+      </c>
+      <c r="H11" s="8">
+        <v>7</v>
+      </c>
+      <c r="I11" s="8">
+        <v>8</v>
+      </c>
+      <c r="J11" s="8">
+        <v>9</v>
+      </c>
+      <c r="K11" s="8">
+        <v>10</v>
+      </c>
+      <c r="L11" s="8">
+        <v>11</v>
+      </c>
+      <c r="M11" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="15"/>
+</worksheet>
 </file>
</xml_diff>